<commit_message>
Update TitanX numbers for TN gemm case.
</commit_message>
<xml_diff>
--- a/results/DeepBench_NV_TitanX.xlsx
+++ b/results/DeepBench_NV_TitanX.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27430"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="560" yWindow="0" windowWidth="25040" windowHeight="17460" tabRatio="500"/>
+    <workbookView xWindow="560" yWindow="0" windowWidth="29860" windowHeight="19160" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Results" sheetId="1" r:id="rId1"/>
@@ -325,8 +325,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="41">
+  <cellStyleXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -387,7 +389,7 @@
     </xf>
     <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="41">
+  <cellStyles count="43">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -408,6 +410,7 @@
     <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -428,6 +431,7 @@
     <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -759,8 +763,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AC207"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" topLeftCell="A169" workbookViewId="0">
-      <selection activeCell="A197" sqref="A197:XFD197"/>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="B39" workbookViewId="0">
+      <selection activeCell="E57" sqref="E57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2189,11 +2193,11 @@
         <v>2</v>
       </c>
       <c r="I56">
-        <v>74.676000000000002</v>
+        <v>56.341999999999999</v>
       </c>
       <c r="J56" s="1">
         <f t="shared" si="0"/>
-        <v>2.2037179752530931</v>
+        <v>2.9208200546661458</v>
       </c>
       <c r="K56" s="10"/>
       <c r="L56" s="1"/>
@@ -2215,11 +2219,11 @@
         <v>2</v>
       </c>
       <c r="I57">
-        <v>0.6</v>
+        <v>0.66600000000000004</v>
       </c>
       <c r="J57" s="1">
         <f t="shared" si="0"/>
-        <v>1.7365040000000003</v>
+        <v>1.5644180180180178</v>
       </c>
       <c r="K57" s="10"/>
       <c r="L57" s="1"/>
@@ -2241,11 +2245,11 @@
         <v>2</v>
       </c>
       <c r="I58">
-        <v>71.745999999999995</v>
+        <v>40.795999999999999</v>
       </c>
       <c r="J58" s="1">
         <f t="shared" si="0"/>
-        <v>2.6690496487051547</v>
+        <v>4.6939316623198346</v>
       </c>
       <c r="K58" s="10"/>
       <c r="L58" s="1"/>
@@ -2267,11 +2271,11 @@
         <v>2</v>
       </c>
       <c r="I59">
-        <v>0.58099999999999996</v>
+        <v>0.73899999999999999</v>
       </c>
       <c r="J59" s="1">
         <f t="shared" si="0"/>
-        <v>2.0867392771084341</v>
+        <v>1.6405893369418132</v>
       </c>
       <c r="K59" s="10"/>
       <c r="L59" s="1"/>
@@ -2293,11 +2297,11 @@
         <v>2</v>
       </c>
       <c r="I60">
-        <v>95.858000000000004</v>
+        <v>85.013000000000005</v>
       </c>
       <c r="J60" s="1">
         <f t="shared" si="0"/>
-        <v>2.4971003475974878</v>
+        <v>2.8156522545963556</v>
       </c>
       <c r="K60" s="10"/>
       <c r="L60" s="1"/>
@@ -2319,11 +2323,11 @@
         <v>2</v>
       </c>
       <c r="I61">
-        <v>0.72</v>
+        <v>0.92</v>
       </c>
       <c r="J61" s="1">
         <f t="shared" si="0"/>
-        <v>2.1048533333333337</v>
+        <v>1.6472765217391303</v>
       </c>
       <c r="K61" s="10"/>
       <c r="L61" s="1"/>
@@ -2345,11 +2349,11 @@
         <v>2</v>
       </c>
       <c r="I62">
-        <v>153</v>
+        <v>92.891000000000005</v>
       </c>
       <c r="J62" s="1">
         <f t="shared" si="0"/>
-        <v>2.5031847855686276</v>
+        <v>4.1229750157927034</v>
       </c>
       <c r="K62" s="10"/>
       <c r="L62" s="1"/>
@@ -2371,11 +2375,11 @@
         <v>2</v>
       </c>
       <c r="I63">
-        <v>1.161</v>
+        <v>1.444</v>
       </c>
       <c r="J63" s="1">
         <f t="shared" si="0"/>
-        <v>2.0885366408268728</v>
+        <v>1.6792181717451524</v>
       </c>
       <c r="K63" s="10"/>
       <c r="L63" s="1"/>
@@ -2506,11 +2510,11 @@
         <v>2</v>
       </c>
       <c r="I69">
-        <v>0.84099999999999997</v>
+        <v>0.84599999999999997</v>
       </c>
       <c r="J69" s="1">
         <f t="shared" si="1"/>
-        <v>0.74809227110582643</v>
+        <v>0.74367092198581564</v>
       </c>
       <c r="K69" s="10"/>
       <c r="L69" s="1"/>
@@ -2532,11 +2536,11 @@
         <v>2</v>
       </c>
       <c r="I70">
-        <v>0.84599999999999997</v>
+        <v>0.85</v>
       </c>
       <c r="J70" s="1">
         <f t="shared" si="1"/>
-        <v>1.4873418439716313</v>
+        <v>1.4803425882352943</v>
       </c>
       <c r="K70" s="10"/>
       <c r="L70" s="1"/>
@@ -2558,11 +2562,11 @@
         <v>2</v>
       </c>
       <c r="I71">
-        <v>1.754</v>
+        <v>1.4850000000000001</v>
       </c>
       <c r="J71" s="1">
         <f t="shared" si="1"/>
-        <v>1.4347676168757126</v>
+        <v>1.6946682828282829</v>
       </c>
       <c r="K71" s="10"/>
       <c r="L71" s="1"/>
@@ -2584,11 +2588,11 @@
         <v>2</v>
       </c>
       <c r="I72">
-        <v>1.78</v>
+        <v>2.2149999999999999</v>
       </c>
       <c r="J72" s="1">
         <f t="shared" si="1"/>
-        <v>2.8276206741573033</v>
+        <v>2.2723091647855531</v>
       </c>
       <c r="K72" s="10"/>
       <c r="L72" s="1"/>
@@ -2719,11 +2723,11 @@
         <v>2</v>
       </c>
       <c r="I77">
-        <v>0.152</v>
+        <v>0.216</v>
       </c>
       <c r="J77" s="1">
         <f t="shared" si="1"/>
-        <v>0.66225852631578941</v>
+        <v>0.46603377777777777</v>
       </c>
       <c r="K77" s="10"/>
       <c r="L77" s="1"/>
@@ -2746,11 +2750,11 @@
         <v>2</v>
       </c>
       <c r="I78">
-        <v>0.154</v>
+        <v>0.217</v>
       </c>
       <c r="J78" s="1">
         <f t="shared" si="1"/>
-        <v>1.3073155324675325</v>
+        <v>0.9277723133640553</v>
       </c>
       <c r="K78" s="10"/>
       <c r="L78" s="1"/>
@@ -2773,11 +2777,11 @@
         <v>2</v>
       </c>
       <c r="I79">
-        <v>0.376</v>
+        <v>0.19900000000000001</v>
       </c>
       <c r="J79" s="1">
         <f t="shared" si="1"/>
-        <v>1.0708861276595747</v>
+        <v>2.0233828341708544</v>
       </c>
       <c r="K79" s="10"/>
       <c r="L79" s="1"/>
@@ -2800,11 +2804,11 @@
         <v>2</v>
       </c>
       <c r="I80">
-        <v>0.59699999999999998</v>
+        <v>0.224</v>
       </c>
       <c r="J80" s="1">
         <f t="shared" si="1"/>
-        <v>1.3489218894472363</v>
+        <v>3.5951177142857142</v>
       </c>
       <c r="K80" s="10"/>
       <c r="L80" s="1"/>

</xml_diff>